<commit_message>
Update to lob in more explicit stuff about the admin interface
</commit_message>
<xml_diff>
--- a/Blank-IoT_CheckList.xlsx
+++ b/Blank-IoT_CheckList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18864" yWindow="0" windowWidth="13368" windowHeight="5292" activeTab="1"/>
+    <workbookView xWindow="20652" yWindow="0" windowWidth="13368" windowHeight="5292"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -264,6 +264,30 @@
     <t xml:space="preserve">For each of the 10 points that are the responsibility of developers. Consider your implementation. 
 At this point the LoRa specification is relatively young in networking protocol terms. In Secarma’s experience this would mean that more flaws are likely overtime. 
 Providing a robust means of update as recommended under general technical concerns should allow your device to patch against implementation flaws. However, if the protocol is proved insecure in the manner of early Wi-Fi networks (e.g. WEP). Then patching will likely not be enough and devices would essentially be insecure and obsolete.
+</t>
+  </si>
+  <si>
+    <t>Insecure Web Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most devices offer some form of web application to provision and administer the device. These interfaces are vulnerable to the same risks as enterprise applications or Internet sites. However, it is true that IoT admin interfaces have not been generally subjected to the same security assessment as those more familiar targets.
+In fact, it is true that these admin interfaces are at increased risk of attack because the owner of the device has physical access. As such the firmware can be retrieved which includes the code for the web application. Attackers have time to sift through this code to find weaknesses while they do not have this luxury for traditional web sites in most cases.
+Common web application flaws in embedded admin interfaces include:
+• Remote code execution
+• Local/Remote File Includes
+• Directory Traversal
+• Cross Site Scripting (XSS)
+• Denial of Service
+Every application level flaw is applicable but these are likely within IoT admin interfaces.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educate developers on the risks of common web application flaws. Security engaged engineers are effective to limit risks.
+Leverage static code review tools which may help you locate flaws early.
+However, it is also key to have your administration applications assessed by a trusted 3rd party. This should not be an automated vulnerability assessment it needs to include manual assessment to find the best results.
+To make this process as cost effective as possible we would recommend providing the source code for the interface along with access to the underlying operating system. 
+To ensure coverage it is best to start from a position of knowing every file accessible via the web server. Thinking that someone will “never find” content that is not linked to directly is wrong in this case. Since the firmware will be accessible the attacker will have access anyway if they look in the right places.
+While classic web application testing is the skillset required. For the purposes of embedded devices it is best to provide as much information as possible so the audit can be comprehensive.
 </t>
   </si>
 </sst>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,45 +787,59 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="289.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="6" spans="1:4" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="168" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+    <row r="7" spans="1:4" ht="168" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -815,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>